<commit_message>
cleaned code; add readme
</commit_message>
<xml_diff>
--- a/reports/nn_mod_1/banknote-authentication_nf_4/xc7z010clg400-1/Table.xlsx
+++ b/reports/nn_mod_1/banknote-authentication_nf_4/xc7z010clg400-1/Table.xlsx
@@ -147,13 +147,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>72716.0</v>
+        <v>8914.0</v>
       </c>
       <c r="C2" t="n" s="4">
         <v>17600.0</v>
       </c>
       <c r="D2" t="n" s="6">
-        <v>413.1590881347656</v>
+        <v>50.647727966308594</v>
       </c>
     </row>
     <row r="3">
@@ -175,13 +175,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n" s="4">
-        <v>50156.0</v>
+        <v>11715.0</v>
       </c>
       <c r="C4" t="n" s="4">
         <v>35200.0</v>
       </c>
       <c r="D4" t="n" s="6">
-        <v>142.48863220214844</v>
+        <v>33.28125</v>
       </c>
     </row>
     <row r="5">
@@ -203,13 +203,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n" s="4">
-        <v>80.0</v>
+        <v>78.0</v>
       </c>
       <c r="C6" t="n" s="4">
         <v>80.0</v>
       </c>
       <c r="D6" t="n" s="6">
-        <v>100.0</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="7">

</xml_diff>